<commit_message>
Updating NuGet packages and valid TestData dates + demo video.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sprint3.nunit\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\prodesk\projects\sprint3.nunit\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548"/>
   </bookViews>
   <sheets>
     <sheet name="ShareSkill" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Url</t>
   </si>
@@ -199,9 +199,6 @@
     <t>MS Word</t>
   </si>
   <si>
-    <t>31/09/2022</t>
-  </si>
-  <si>
     <t>Testing 123... for deletion anyway.</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>wsample5.png</t>
+  </si>
+  <si>
+    <t>31/11/2022</t>
   </si>
 </sst>
 </file>
@@ -617,28 +617,28 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -685,7 +685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -708,10 +708,10 @@
         <v>38</v>
       </c>
       <c r="H2" s="8">
-        <v>44752</v>
-      </c>
-      <c r="I2" s="5">
-        <v>44804</v>
+        <v>44844</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="J2" s="6">
         <v>0.29166666666666669</v>
@@ -726,13 +726,13 @@
         <v>30</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
@@ -749,16 +749,16 @@
         <v>52</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="8">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="I3" s="5">
-        <v>44804</v>
+        <v>44865</v>
       </c>
       <c r="J3" s="6">
         <v>0.33333333333333331</v>
@@ -773,13 +773,13 @@
         <v>25</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
@@ -802,10 +802,10 @@
         <v>38</v>
       </c>
       <c r="H4" s="8">
-        <v>44774</v>
+        <v>44835</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="J4" s="6">
         <v>0.41666666666666669</v>
@@ -820,16 +820,16 @@
         <v>20</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>55</v>
@@ -841,16 +841,16 @@
         <v>57</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H5" s="8">
-        <v>44805</v>
-      </c>
-      <c r="I5" s="5">
-        <v>44865</v>
+        <v>44835</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="J5" s="6">
         <v>0.375</v>
@@ -865,18 +865,18 @@
         <v>20</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>55</v>
@@ -892,10 +892,10 @@
         <v>38</v>
       </c>
       <c r="H6" s="8">
-        <v>44806</v>
+        <v>44867</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="J6" s="6">
         <v>0.33333333333333331</v>
@@ -910,18 +910,18 @@
         <v>20</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>55</v>
@@ -933,7 +933,7 @@
         <v>57</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>38</v>
@@ -957,7 +957,7 @@
         <v>20</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>32</v>
@@ -977,25 +977,25 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1042,12 +1042,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>46</v>
@@ -1068,15 +1068,15 @@
       <selection activeCell="E19" sqref="A13:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1124,14 +1124,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1167,19 +1167,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="1" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Destructive testing for Adding ShareSkill. Also correcting filename from 'TC_014_ShareSkills_AddNew' to 'TC_013_ShareSkills_AddNew' to sync with documentation.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\prodesk\projects\sprint3.nunit\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sprint3\sprint3.nunit\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>Url</t>
   </si>
@@ -157,9 +157,6 @@
     <t>End time</t>
   </si>
   <si>
-    <t>Develop test automation scripts with a specialization in C Sharp, Selenium and other tools.</t>
-  </si>
-  <si>
     <t>Quality Assurance</t>
   </si>
   <si>
@@ -169,12 +166,6 @@
     <t>Skill-exchanges</t>
   </si>
   <si>
-    <t>3D Animator</t>
-  </si>
-  <si>
-    <t>Video editing and 3D animation.</t>
-  </si>
-  <si>
     <t>Video &amp; Animation</t>
   </si>
   <si>
@@ -184,9 +175,6 @@
     <t>3D Studiomax</t>
   </si>
   <si>
-    <t>Design and create media advertisements.</t>
-  </si>
-  <si>
     <t>Copy Writer</t>
   </si>
   <si>
@@ -205,41 +193,32 @@
     <t>One-off service</t>
   </si>
   <si>
-    <t>wsample3.png</t>
-  </si>
-  <si>
     <t>worksample.txt</t>
   </si>
   <si>
-    <t>wsample2.png</t>
-  </si>
-  <si>
-    <t>fileupload_x64.exe</t>
-  </si>
-  <si>
-    <t>Missing title</t>
-  </si>
-  <si>
-    <t>Unslected Subcategory</t>
-  </si>
-  <si>
-    <t>Invalid file type upload</t>
-  </si>
-  <si>
-    <t>wsample4.png</t>
-  </si>
-  <si>
-    <t>wsample5.png</t>
-  </si>
-  <si>
-    <t>31/11/2022</t>
+    <t>Upload invalid file type and size</t>
+  </si>
+  <si>
+    <t>InvalidTypeAndSize.mp4</t>
+  </si>
+  <si>
+    <t>wsample.png</t>
+  </si>
+  <si>
+    <t>hack test &lt;script&gt;alert("YOU GOT HACKED by Javascript injection!");&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>Test Automation using Selenium with C Sharp along with other testing frameworks and tools.</t>
+  </si>
+  <si>
+    <t>Injecting Javascript or Malicious title along with special or invalid special characters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +229,14 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -295,9 +282,6 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -309,6 +293,15 @@
     </xf>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,83 +607,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="4" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>34</v>
@@ -707,11 +701,13 @@
       <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="8">
-        <v>44844</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>69</v>
+      <c r="H2" s="7">
+        <f ca="1">TODAY()+CHOOSE(RANDBETWEEN(1, 6), 5, 9, 15, 17, 21, 27)</f>
+        <v>44832</v>
+      </c>
+      <c r="I2" s="5">
+        <f ca="1">H2+CHOOSE(RANDBETWEEN(1,6),8,12,16,22,26,30)</f>
+        <v>44862</v>
       </c>
       <c r="J2" s="6">
         <v>0.29166666666666669</v>
@@ -719,46 +715,48 @@
       <c r="K2" s="6">
         <v>0.625</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="4">
+      <c r="L2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="13">
         <v>30</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="8">
-        <v>44835</v>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H4" ca="1" si="0">TODAY()+CHOOSE(RANDBETWEEN(1, 6), 5, 9, 15, 17, 21, 27)</f>
+        <v>44832</v>
       </c>
       <c r="I3" s="5">
-        <v>44865</v>
+        <f t="shared" ref="I3:I4" ca="1" si="1">H3+CHOOSE(RANDBETWEEN(1,6),8,12,16,22,26,30)</f>
+        <v>44854</v>
       </c>
       <c r="J3" s="6">
         <v>0.33333333333333331</v>
@@ -766,200 +764,65 @@
       <c r="K3" s="6">
         <v>0.66666666666666663</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="L3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="13">
         <v>25</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="8">
-        <v>44835</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>69</v>
+      <c r="H4" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44840</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>44852</v>
       </c>
       <c r="J4" s="6">
-        <v>0.41666666666666669</v>
+        <v>0.3125</v>
       </c>
       <c r="K4" s="6">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="4">
+        <v>0.6875</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="13">
         <v>20</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="8">
-        <v>44835</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0.375</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="4">
-        <v>20</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="8">
-        <v>44867</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="4">
-        <v>20</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="8">
-        <v>44869</v>
-      </c>
-      <c r="I7" s="5">
-        <v>44926</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0.3125</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0.6875</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="4">
-        <v>20</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="O7" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1042,18 +905,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:15" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>